<commit_message>
Atualização do Roadmap de cruds basicos
</commit_message>
<xml_diff>
--- a/Documentação/Controle de Cruds.xlsx
+++ b/Documentação/Controle de Cruds.xlsx
@@ -360,55 +360,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,7 +693,7 @@
   <dimension ref="B2:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,17 +707,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -727,10 +728,10 @@
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
@@ -748,36 +749,36 @@
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -787,10 +788,10 @@
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -800,23 +801,23 @@
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -826,10 +827,10 @@
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -839,10 +840,10 @@
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -852,10 +853,10 @@
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -865,57 +866,52 @@
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="4"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
     <row r="16" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="16"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="14"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C16:H17"/>
@@ -927,6 +923,11 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Login mobile e Desktop
</commit_message>
<xml_diff>
--- a/Documentação/Controle de Cruds.xlsx
+++ b/Documentação/Controle de Cruds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\sites\unibr-tcc-ads\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrunoAlves\htdocs\faculdade\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -368,6 +368,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -395,22 +411,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,31 +694,31 @@
   <dimension ref="B2:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.125" customWidth="1"/>
+    <col min="3" max="3" width="9.125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="17.875" customWidth="1"/>
     <col min="5" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -729,10 +729,10 @@
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="20"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
@@ -750,10 +750,10 @@
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -763,10 +763,10 @@
       <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="13"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -776,10 +776,10 @@
       <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -789,10 +789,10 @@
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -802,23 +802,23 @@
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -828,10 +828,10 @@
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -841,23 +841,31 @@
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="2">
+        <v>80</v>
+      </c>
+      <c r="F11" s="2">
+        <v>90</v>
+      </c>
+      <c r="G11" s="2">
+        <v>90</v>
+      </c>
+      <c r="H11" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -867,10 +875,10 @@
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="5"/>
       <c r="F13" s="6"/>
       <c r="G13" s="5"/>
@@ -880,44 +888,39 @@
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
     <row r="16" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="10"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="13"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C16:H17"/>
@@ -929,6 +932,11 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>